<commit_message>
Commit from Develop branch
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/TestData.xlsx
+++ b/src/test/resources/excel/TestData.xlsx
@@ -3,23 +3,24 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sayan\IdeaProjects\DataDrivenApproch\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38EE04CE-D23B-492F-AC6E-B5C2459042DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0D7BC8-2E65-4589-8058-C9D994C74497}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateDeleteCustFunctionality" sheetId="5" r:id="rId1"/>
-    <sheet name="OpenAccountFunctionality" sheetId="2" r:id="rId2"/>
-    <sheet name="DepositWithdrawFunctionality" sheetId="4" r:id="rId3"/>
+    <sheet name="DifferentActions" sheetId="6" r:id="rId2"/>
+    <sheet name="OpenAccountFunctionality" sheetId="2" r:id="rId3"/>
+    <sheet name="DepositWithdrawFunctionality" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="57">
   <si>
     <t>TC Name</t>
   </si>
@@ -188,17 +189,28 @@
     <t>500</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Fail</t>
+  </si>
+  <si>
+    <t>Window_Authorization</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>Upload_File_Using_Send_Keys</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -513,18 +525,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AF64476-F0D0-4FE1-B4B7-91EF5B62511E}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="52.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="1" max="1" width="52.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -588,7 +600,7 @@
       </c>
       <c r="E3" s="1"/>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G3" t="s">
         <v>45</v>
@@ -615,6 +627,68 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C96219E-A347-4014-A376-320CB641BFF2}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ADD4165-CA4F-4CA3-87F9-D6761A1072F6}">
   <dimension ref="A1:H4"/>
   <sheetViews>
@@ -624,12 +698,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="56.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="1" max="1" width="56.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -742,7 +816,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3B70980-4E13-4015-96B1-5FDB52014543}">
   <dimension ref="A1:I10"/>
   <sheetViews>
@@ -752,14 +826,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="7.85546875" collapsed="true"/>
-    <col min="6" max="7" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -868,7 +942,7 @@
         <v>42</v>
       </c>
       <c r="H5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I5" t="s">
         <v>45</v>

</xml_diff>